<commit_message>
Mo working on dialogs
</commit_message>
<xml_diff>
--- a/Wi-UI.xlsx
+++ b/Wi-UI.xlsx
@@ -19,7 +19,7 @@
     <sheet name="WorkingBlock" sheetId="10" r:id="rId10"/>
     <sheet name="Dialogs" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="144525" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="325">
   <si>
     <t>Code</t>
   </si>
@@ -1004,6 +1004,9 @@
   </si>
   <si>
     <t>DataProcessing</t>
+  </si>
+  <si>
+    <t>confirm dialog</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1440,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1756,10 +1759,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,7 +1772,7 @@
     <col min="3" max="3" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>321</v>
       </c>
@@ -1780,14 +1783,14 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>SUBSTITUTE(CONCATENATE(B3,"Modal")," ","")</f>
         <v>NewProjectModal</v>
@@ -1799,7 +1802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>SUBSTITUTE(CONCATENATE(B4,"Modal")," ","")</f>
         <v>OpenProjectModal</v>
@@ -1811,7 +1814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>SUBSTITUTE(CONCATENATE(B5,"Modal")," ","")</f>
         <v>CloseProjectModal</v>
@@ -1820,10 +1823,13 @@
         <v>30</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>SUBSTITUTE(CONCATENATE(B6,"Modal")," ","")</f>
         <v>UnitSettingsModal</v>
@@ -1832,10 +1838,10 @@
         <v>32</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>SUBSTITUTE(CONCATENATE(B7,"Modal")," ","")</f>
         <v>ExitModal</v>
@@ -1846,15 +1852,18 @@
       <c r="C7" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" ref="A9:A30" si="0">SUBSTITUTE(CONCATENATE(B9,"Modal")," ","")</f>
         <v>AddNewModal</v>
@@ -1863,7 +1872,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>WellHeaderModal</v>
@@ -1872,7 +1881,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>DepthConversionModal</v>
@@ -1881,7 +1890,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>CurveAliasModal</v>
@@ -1890,7 +1899,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>FamilyEditModal</v>
@@ -1899,7 +1908,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Input/OutputModal</v>
@@ -1908,7 +1917,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>ImportASCIIModal</v>
@@ -1917,7 +1926,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>ImportMultiASCIIModal</v>

</xml_diff>

<commit_message>
curve average update dialog
</commit_message>
<xml_diff>
--- a/Wi-UI.xlsx
+++ b/Wi-UI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="993" activeTab="4"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="993" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="335">
   <si>
     <t>Code</t>
   </si>
@@ -1034,6 +1034,9 @@
   </si>
   <si>
     <t>icon-left</t>
+  </si>
+  <si>
+    <t>Curve Comparison</t>
   </si>
 </sst>
 </file>
@@ -1546,7 +1549,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5019,14 +5022,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
     <col min="8" max="8" width="19.28515625" customWidth="1"/>
@@ -7410,13 +7413,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
@@ -8032,7 +8036,7 @@
       </c>
       <c r="B20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>CurveComrarisonButton</v>
+        <v>CurveComparisonButton</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -8049,7 +8053,7 @@
         <v>curve-compare-16x16</v>
       </c>
       <c r="G20" t="s">
-        <v>240</v>
+        <v>334</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>329</v>

</xml_diff>